<commit_message>
Added delay-disabler.js which should fix the periodic delay bug, added survey related images, updated project log and milestone submission
</commit_message>
<xml_diff>
--- a/Skylab documents/Project Log.xlsx
+++ b/Skylab documents/Project Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\Y1 Summer\Panopto Project\Skylab documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D7A55CA-F8F3-4AE5-9327-D9D48E1F6874}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89108752-0466-4CE2-B992-9EF842B18B76}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="5480" xr2:uid="{18F59187-B1E2-45ED-BF88-DDFCC51EE406}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="48">
   <si>
     <t>Project Log</t>
   </si>
@@ -161,6 +161,76 @@
   </si>
   <si>
     <t>1) Worked on Milestone 1 deliverables (document, video and poster)</t>
+  </si>
+  <si>
+    <t>Team Meeting</t>
+  </si>
+  <si>
+    <t>1) Run through current state of project
+2) Crash course into HTML/CSS &amp; JS for Fyonn</t>
+  </si>
+  <si>
+    <t>1) Basic implementation of audio webworklet for FFT processing with window size of 512 samples.</t>
+  </si>
+  <si>
+    <t>1) Converted use of Promises to async/await for code clarity in webworklet &amp; subtitles.js
+2) Researched on TextTracks cues system
+3) Fixed subtitles bug involving Panopto's desynced two videos system (videos play at different offsets at different timings, only synced at runtime in implementation. Our implementation must thus also be synced at runtime)</t>
+  </si>
+  <si>
+    <t>1) Voice Activity Detection research (https://www.ncbi.nlm.nih.gov/pmc/articles/PMC4142156/)
+1.1) A TLDR on the paper: FFT to get magnitude of frequency bins, then FFT the magnitudes to get the "harmonic information in speech signals". Subsequently calculate the mean frequency bin index (Fmean) and the slope linear regression coefficients for both low index (0 to Fmean) and high index (Fmean to max). These calculated variables (Fmean and the coefficients) form the five-dimensional feature set that defines a "signal". So what it does is get the feature set of a slice of data that is assumed to be noise (which this app assumes to be the first 100ms). This feature set is defined as the reference feature. All subsequent feature sets are compared against this reference to test if they are "speech" or "noise". This comparison is done by taking the difference between each feature set and squashing it down to a single value (referred to as "distance" in the paper as well as in later parts of this project log)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) Re-implementation of VAD based on paper (this sentence hides a lot of the implementation details involving DCFT and other optimizations, but it's basically what the paper describes in javascript, pre-calculated data and a few app-specific tweaks to minimize calculations); involved restructuring of ts-tracker &amp; vad-audio-worklet-processor for inter-thread communications.
+2) Completion of re-implementation and testing. Testing reveals that the noise - voice threshold (the distance value that determines if the signal at that point is "noise" or "voice") varies across different webcasts beyond what the paper has described. </t>
+  </si>
+  <si>
+    <t>1) Implemented silence detection using TextTracks oncuechange (cues system)
+2) Brainstorming for seeking videos (need to keep videos in sync)
+3) Discovered bug involving lag when seeking, bug appears to be involving buffering with HLSJS
+4) More research into Panopto's implementation, HLS.js documentation on their API, Debugging
+5) Implemented basic implementation of silence detection
+6) Potential of silence detection appears very promising. The webcast can be significantly shortened even mid-speech without impacting voice quality.</t>
+  </si>
+  <si>
+    <t>1) 1st attempt to dynamically obtain noise-voice threshold involves using an order statistic tree built on a Binary Indexed Tree (BIT) in order to get the value at the 25th percentile (or a similar method to avoid extreme outliers) and set that value as the threshold. Implementation deemed irrelevant after thought experiments reveal that the distribution of distances may be skewed towards speech / non-speech.
+2) Further thought experiments reveal that it may be more likely that the distribution of distances may follow a bimodal distribution (given that there's two states of "noise" and "no noise", and speech by a professor is likely to be restricted to a range of frequencies). 
+3) Checked this possibility by shifting the data out into a csv file and then plotting the histogram(s) of ~6 minutes long samples from multiple webcasts at different timings (x-axis: difference, y-axis: frequency of data occurance), as well as graphing distance against time using R. No conclusion can be made yet until more webcasts by different professors (and in different venues) have been sampled.
+4) Finished developmental work which allows for testing of thresholds</t>
+  </si>
+  <si>
+    <t>Documentation</t>
+  </si>
+  <si>
+    <t>1) Observation shows that assumption that webcasts start with noise is unwarranted. Discovered some webcasts that start immediately with speech. Changed code to analyse the last TS file instead, and to only analyze the last section of the TS file. If the TS file is too short, use second last. Ignores last second of the webcast as the last second's video and presumably audio is faded out by Panopto.
+2) Voice Activity Detection (VAD) is now officially complete! Program now retrieves 30 samples of noise as the reference sample and build mean &amp; std dev for each of the 5 variables. Using an arbitrary confidence level of 97.8% (based on some experimentation) for all variables, and majority of variables must exceed this confidence level for the signal to be defined as "non-noise". Seems to work well for all webcasts tested. Greater in-depth testing is needed for user satisfaction.
+3) Further analysis on how Panopto sync streams reveals clues on implementation. Desync issue (from jumping too much) resolved with a solution that combines efficiency &amp; desync resistance. 
+4) Added logger-disabler.js to disable logs produced by Panopto's code (to be fair, code in production shouldn't be producing logs...)</t>
+  </si>
+  <si>
+    <t>1) Worked on Milestone 1 deliverables (peer reviewing of documents)</t>
+  </si>
+  <si>
+    <t>1) Restructuring, removing irrelevant files, creating JSDocs &amp; documentation
+2) Modifying README.md, adding package.json to facilitate JSDocs &amp; webpack for distribution</t>
+  </si>
+  <si>
+    <t>Survey</t>
+  </si>
+  <si>
+    <t>Milestone 2 Deliverables</t>
+  </si>
+  <si>
+    <t>1) Work on the Readme.md</t>
+  </si>
+  <si>
+    <t>1) Preparation and release of survey for UI</t>
+  </si>
+  <si>
+    <t>1) Further analysis on Panopto API
+2) Quickfix of the delay bug (implemented in delay-disabler.js), where Panopto has this issue of periodically pausing their player for no noticeable reason
+3) Properly enabled LoggerDisabler</t>
   </si>
 </sst>
 </file>
@@ -556,10 +626,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D66DA078-28E1-44A0-8117-A67A05B0BE09}">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -901,35 +971,256 @@
         <v>6</v>
       </c>
       <c r="E20" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F20" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="C21" s="2" t="s">
+    <row r="21" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="B21" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21" s="9">
+        <v>43616</v>
+      </c>
+      <c r="D21" s="2">
+        <v>6</v>
+      </c>
+      <c r="E21" s="2">
+        <v>6</v>
+      </c>
+      <c r="F21" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B22" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22" s="9">
+        <v>43609</v>
+      </c>
+      <c r="D22" s="2">
+        <v>0</v>
+      </c>
+      <c r="E22" s="2">
+        <v>4</v>
+      </c>
+      <c r="F22" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="B23" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" s="9">
+        <v>43625</v>
+      </c>
+      <c r="D23" s="2">
+        <v>10</v>
+      </c>
+      <c r="E23" s="2">
+        <v>0</v>
+      </c>
+      <c r="F23" s="11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" ht="87" x14ac:dyDescent="0.35">
+      <c r="B24" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24" s="9">
+        <v>43626</v>
+      </c>
+      <c r="D24" s="2">
+        <v>6</v>
+      </c>
+      <c r="E24" s="2">
+        <v>0</v>
+      </c>
+      <c r="F24" s="11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" ht="145" x14ac:dyDescent="0.35">
+      <c r="B25" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C25" s="9">
+        <v>43627</v>
+      </c>
+      <c r="D25" s="2">
+        <v>10</v>
+      </c>
+      <c r="E25" s="2">
+        <v>0</v>
+      </c>
+      <c r="F25" s="11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" ht="217.5" x14ac:dyDescent="0.35">
+      <c r="B26" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C26" s="9">
+        <v>43628</v>
+      </c>
+      <c r="D26" s="2">
+        <v>6</v>
+      </c>
+      <c r="E26" s="2">
+        <v>0</v>
+      </c>
+      <c r="F26" s="11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="B27" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C27" s="9">
+        <v>43629</v>
+      </c>
+      <c r="D27" s="2">
+        <v>10</v>
+      </c>
+      <c r="E27" s="2">
+        <v>0</v>
+      </c>
+      <c r="F27" s="11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" ht="246.5" x14ac:dyDescent="0.35">
+      <c r="B28" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C28" s="9">
+        <v>43637</v>
+      </c>
+      <c r="D28" s="2">
+        <v>10</v>
+      </c>
+      <c r="E28" s="2">
+        <v>0</v>
+      </c>
+      <c r="F28" s="11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" ht="261" x14ac:dyDescent="0.35">
+      <c r="B29" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C29" s="9">
+        <v>43638</v>
+      </c>
+      <c r="D29" s="2">
+        <v>10</v>
+      </c>
+      <c r="E29" s="2">
+        <v>0</v>
+      </c>
+      <c r="F29" s="11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B30" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C30" s="9">
+        <v>43640</v>
+      </c>
+      <c r="D30" s="2">
+        <v>7</v>
+      </c>
+      <c r="E30" s="2">
+        <v>0</v>
+      </c>
+      <c r="F30" s="11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B31" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C31" s="9">
+        <v>43641</v>
+      </c>
+      <c r="D31" s="2">
+        <v>4</v>
+      </c>
+      <c r="E31" s="2">
+        <v>0</v>
+      </c>
+      <c r="F31" s="11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B32" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C32" s="9">
+        <v>43641</v>
+      </c>
+      <c r="D32" s="2">
+        <v>2</v>
+      </c>
+      <c r="E32" s="2">
+        <v>0</v>
+      </c>
+      <c r="F32" s="11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="B33" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C33" s="9">
+        <v>43641</v>
+      </c>
+      <c r="D33" s="2">
+        <v>2</v>
+      </c>
+      <c r="E33" s="2">
+        <v>0</v>
+      </c>
+      <c r="F33" s="11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C42" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D42" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E21" s="3" t="s">
+      <c r="E42" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="C22" s="1">
-        <f>SUM(D3:E20)</f>
-        <v>122</v>
-      </c>
-      <c r="D22" s="2">
-        <f>SUM(D3:D20)</f>
-        <v>112</v>
-      </c>
-      <c r="E22" s="2">
-        <f>SUM(E3:E20)</f>
-        <v>10</v>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C43" s="1">
+        <f>SUM(D43:E43)</f>
+        <v>214</v>
+      </c>
+      <c r="D43" s="2">
+        <f>SUM(D3:D42)</f>
+        <v>195</v>
+      </c>
+      <c r="E43" s="2">
+        <f>SUM(E3:E42)</f>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modifications to delay-disabler.js to make it better by directly setting the playstate and also directly making the video run. Also modifications to silence cue manager console log and ts tracker to prevent loading duplicates.
</commit_message>
<xml_diff>
--- a/Skylab documents/Project Log.xlsx
+++ b/Skylab documents/Project Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\Y1 Summer\Panopto Project\Skylab documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89108752-0466-4CE2-B992-9EF842B18B76}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA1BDF92-0D13-49AB-A737-ACE71A74D9B6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="5480" xr2:uid="{18F59187-B1E2-45ED-BF88-DDFCC51EE406}"/>
   </bookViews>
@@ -229,7 +229,7 @@
   </si>
   <si>
     <t>1) Further analysis on Panopto API
-2) Quickfix of the delay bug (implemented in delay-disabler.js), where Panopto has this issue of periodically pausing their player for no noticeable reason
+2) Quickfix of the delay bug (implemented in delay-disabler.js), where Panopto has this issue of periodically pausing their player for no noticeable or intuitive reason (aside from the fact that it is a bug that doesn't surface because it only appears at higher playback speeds)
 3) Properly enabled LoggerDisabler</t>
   </si>
 </sst>
@@ -1181,7 +1181,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="33" spans="2:6" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:6" ht="87" x14ac:dyDescent="0.35">
       <c r="B33" s="10" t="s">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
fixed subtitle sync, updated project log (still need to update)
</commit_message>
<xml_diff>
--- a/Skylab documents/Project Log.xlsx
+++ b/Skylab documents/Project Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\Y1 Summer\Panopto Project\Skylab documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA1BDF92-0D13-49AB-A737-ACE71A74D9B6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E3C9443-112E-483C-B3F1-34EE6FB0368C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="5480" xr2:uid="{18F59187-B1E2-45ED-BF88-DDFCC51EE406}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="51">
   <si>
     <t>Project Log</t>
   </si>
@@ -231,6 +231,19 @@
     <t>1) Further analysis on Panopto API
 2) Quickfix of the delay bug (implemented in delay-disabler.js), where Panopto has this issue of periodically pausing their player for no noticeable or intuitive reason (aside from the fact that it is a bug that doesn't surface because it only appears at higher playback speeds)
 3) Properly enabled LoggerDisabler</t>
+  </si>
+  <si>
+    <t>27/6/2019 - 
+28/6/2019</t>
+  </si>
+  <si>
+    <t>1) Further developmental work to remove memory leak; re-implemented using a buffering system to reduce amount of threads spawned, but memory leak persisted.
+2) Re-implemented using a web worker instead and analysing the PCM data directly, bypassing the OfflineAudioContext, which fixed memory leak. This had the side effect of making the code more readable.</t>
+  </si>
+  <si>
+    <t>1) Bug fixes across the application with regards to delay-disabler.js and how the application detects if a webcast is single or double video stream etc
+2) In-depth testing of silence removal detects memory leak
+3) Further testing and research reveals that the leak is caused by OfflineAudioContext not being garbage collected</t>
   </si>
 </sst>
 </file>
@@ -274,7 +287,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -311,6 +324,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -628,8 +644,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D66DA078-28E1-44A0-8117-A67A05B0BE09}">
   <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+    <sheetView tabSelected="1" topLeftCell="B30" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1155,7 +1171,7 @@
         <v>43641</v>
       </c>
       <c r="D31" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E31" s="2">
         <v>0</v>
@@ -1198,6 +1214,34 @@
         <v>47</v>
       </c>
     </row>
+    <row r="34" spans="2:6" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="B34" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C34" s="9">
+        <v>43642</v>
+      </c>
+      <c r="D34" s="2">
+        <v>6</v>
+      </c>
+      <c r="F34" s="11" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" ht="87" x14ac:dyDescent="0.35">
+      <c r="B35" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C35" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="D35" s="2">
+        <v>14</v>
+      </c>
+      <c r="F35" s="11" t="s">
+        <v>49</v>
+      </c>
+    </row>
     <row r="42" spans="2:6" x14ac:dyDescent="0.35">
       <c r="C42" s="2" t="s">
         <v>15</v>
@@ -1212,11 +1256,11 @@
     <row r="43" spans="2:6" x14ac:dyDescent="0.35">
       <c r="C43" s="1">
         <f>SUM(D43:E43)</f>
-        <v>214</v>
+        <v>236</v>
       </c>
       <c r="D43" s="2">
         <f>SUM(D3:D42)</f>
-        <v>195</v>
+        <v>217</v>
       </c>
       <c r="E43" s="2">
         <f>SUM(E3:E42)</f>

</xml_diff>

<commit_message>
Finished milestone 2 deliverables, fixed subtitle sync with 2nd implementation, updated project log
</commit_message>
<xml_diff>
--- a/Skylab documents/Project Log.xlsx
+++ b/Skylab documents/Project Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\Y1 Summer\Panopto Project\Skylab documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E3C9443-112E-483C-B3F1-34EE6FB0368C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64112269-3DB9-4F0B-9958-F5D902F72AC5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="5480" xr2:uid="{18F59187-B1E2-45ED-BF88-DDFCC51EE406}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="53">
   <si>
     <t>Project Log</t>
   </si>
@@ -237,13 +237,22 @@
 28/6/2019</t>
   </si>
   <si>
-    <t>1) Further developmental work to remove memory leak; re-implemented using a buffering system to reduce amount of threads spawned, but memory leak persisted.
-2) Re-implemented using a web worker instead and analysing the PCM data directly, bypassing the OfflineAudioContext, which fixed memory leak. This had the side effect of making the code more readable.</t>
-  </si>
-  <si>
     <t>1) Bug fixes across the application with regards to delay-disabler.js and how the application detects if a webcast is single or double video stream etc
 2) In-depth testing of silence removal detects memory leak
 3) Further testing and research reveals that the leak is caused by OfflineAudioContext not being garbage collected</t>
+  </si>
+  <si>
+    <t>30/6/2019 - 
+1/6/2019</t>
+  </si>
+  <si>
+    <t>1) Creating, recording and publishing of video
+2) Creating poster</t>
+  </si>
+  <si>
+    <t>1) Further developmental work to remove memory leak; re-implemented using a buffering system to reduce amount of threads spawned, but memory leak persisted.
+2) Re-implemented using a web worker instead and analysing the PCM data directly, bypassing the OfflineAudioContext, which fixed memory leak. This had the side effect of making the code more readable.
+3) Fixing subtitle sync</t>
   </si>
 </sst>
 </file>
@@ -322,11 +331,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -642,10 +651,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D66DA078-28E1-44A0-8117-A67A05B0BE09}">
-  <dimension ref="A1:F43"/>
+  <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B30" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -659,14 +668,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
+      <c r="A1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
@@ -1224,46 +1233,69 @@
       <c r="D34" s="2">
         <v>6</v>
       </c>
+      <c r="E34" s="2">
+        <v>0</v>
+      </c>
       <c r="F34" s="11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="B35" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C35" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="D35" s="2">
+        <v>15</v>
+      </c>
+      <c r="E35" s="2">
+        <v>0</v>
+      </c>
+      <c r="F35" s="11" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B36" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C36" s="12" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="35" spans="2:6" ht="87" x14ac:dyDescent="0.35">
-      <c r="B35" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C35" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="D35" s="2">
+      <c r="D36" s="2">
+        <v>5</v>
+      </c>
+      <c r="E36" s="2">
+        <v>0</v>
+      </c>
+      <c r="F36" s="11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C37" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E37" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F35" s="11" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="C42" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D42" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E42" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="C43" s="1">
-        <f>SUM(D43:E43)</f>
-        <v>236</v>
-      </c>
-      <c r="D43" s="2">
-        <f>SUM(D3:D42)</f>
-        <v>217</v>
-      </c>
-      <c r="E43" s="2">
-        <f>SUM(E3:E42)</f>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C38" s="1">
+        <f>SUM(D38:E38)</f>
+        <v>242</v>
+      </c>
+      <c r="D38" s="2">
+        <f>SUM(D3:D37)</f>
+        <v>223</v>
+      </c>
+      <c r="E38" s="2">
+        <f>SUM(E3:E37)</f>
         <v>19</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added megalist, added new slider options, removed webpack from package.json, updated project log
</commit_message>
<xml_diff>
--- a/Skylab documents/Project Log.xlsx
+++ b/Skylab documents/Project Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\Y1 Summer\Panopto Project\Skylab documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64112269-3DB9-4F0B-9958-F5D902F72AC5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C083A425-B7FC-4891-9328-E46A2560DB35}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="5480" xr2:uid="{18F59187-B1E2-45ED-BF88-DDFCC51EE406}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="57">
   <si>
     <t>Project Log</t>
   </si>
@@ -242,10 +242,6 @@
 3) Further testing and research reveals that the leak is caused by OfflineAudioContext not being garbage collected</t>
   </si>
   <si>
-    <t>30/6/2019 - 
-1/6/2019</t>
-  </si>
-  <si>
     <t>1) Creating, recording and publishing of video
 2) Creating poster</t>
   </si>
@@ -253,6 +249,37 @@
     <t>1) Further developmental work to remove memory leak; re-implemented using a buffering system to reduce amount of threads spawned, but memory leak persisted.
 2) Re-implemented using a web worker instead and analysing the PCM data directly, bypassing the OfflineAudioContext, which fixed memory leak. This had the side effect of making the code more readable.
 3) Fixing subtitle sync</t>
+  </si>
+  <si>
+    <t>1) Worked on Milestone 2 deliverables (peer reviewing of documents)</t>
+  </si>
+  <si>
+    <t>30/6/2019 - 
+1/7/2019</t>
+  </si>
+  <si>
+    <t>10/7/2019 
+- 11/7/2019</t>
+  </si>
+  <si>
+    <t>1) Fixed subtitle sync
+2) Added icons to sidebar, 
+3) Implemented1 or 2 vid stream sidebar, 
+4) Implemented expiry cache
+5) resizable sidebar implemented
+6) settings page implemented w/ preact
+7) notify.min.js added (popups), 
+8) customizability with settings added
+9) volume booster added
+10) responsiveness added
+11) init.js updated with new App object, 
+12) JSDocs updated
+13) all sorts of customizability with carousel and speed slider implemented (including slider alternatives)</t>
+  </si>
+  <si>
+    <t>1) Reworking subtitles.js to incorporate implementation of transcript display
+2) Started work on displaying transcripts
+3) Work halted because Panopto's SSL certs expired (omg, this is not the first time their system experienced a critical failure this summer…)</t>
   </si>
 </sst>
 </file>
@@ -651,10 +678,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D66DA078-28E1-44A0-8117-A67A05B0BE09}">
-  <dimension ref="A1:F38"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1254,7 +1281,7 @@
         <v>0</v>
       </c>
       <c r="F35" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="36" spans="2:6" ht="43.5" x14ac:dyDescent="0.35">
@@ -1262,7 +1289,7 @@
         <v>44</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D36" s="2">
         <v>5</v>
@@ -1271,32 +1298,83 @@
         <v>0</v>
       </c>
       <c r="F36" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="C37" s="2" t="s">
+      <c r="B37" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C37" s="9">
+        <v>43650</v>
+      </c>
+      <c r="D37" s="2">
+        <v>0</v>
+      </c>
+      <c r="E37" s="2">
+        <v>4</v>
+      </c>
+      <c r="F37" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" ht="203" x14ac:dyDescent="0.35">
+      <c r="B38" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C38" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="D38" s="2">
+        <v>14</v>
+      </c>
+      <c r="E38" s="2">
+        <v>0</v>
+      </c>
+      <c r="F38" s="11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="B39" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C39" s="9">
+        <v>43658</v>
+      </c>
+      <c r="D39" s="2">
+        <v>4</v>
+      </c>
+      <c r="E39" s="2">
+        <v>0</v>
+      </c>
+      <c r="F39" s="11" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C40" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D37" s="3" t="s">
+      <c r="D40" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E37" s="3" t="s">
+      <c r="E40" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="C38" s="1">
-        <f>SUM(D38:E38)</f>
-        <v>242</v>
-      </c>
-      <c r="D38" s="2">
-        <f>SUM(D3:D37)</f>
-        <v>223</v>
-      </c>
-      <c r="E38" s="2">
-        <f>SUM(E3:E37)</f>
-        <v>19</v>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C41" s="1">
+        <f>SUM(D41:E41)</f>
+        <v>264</v>
+      </c>
+      <c r="D41" s="2">
+        <f>SUM(D3:D40)</f>
+        <v>241</v>
+      </c>
+      <c r="E41" s="2">
+        <f>SUM(E3:E40)</f>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
1) Misc fixes like fixes to the minimize / maximize button  2) Added transcript tab on second screen tab  3) Testing  4) Added full-screen option  5) Updated read me
</commit_message>
<xml_diff>
--- a/Skylab documents/Project Log.xlsx
+++ b/Skylab documents/Project Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\Y1 Summer\Panopto Project\Skylab documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C083A425-B7FC-4891-9328-E46A2560DB35}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34E3C5A5-84AB-467C-8CB8-4FD36D2BE704}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="5480" xr2:uid="{18F59187-B1E2-45ED-BF88-DDFCC51EE406}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="62">
   <si>
     <t>Project Log</t>
   </si>
@@ -280,6 +280,31 @@
     <t>1) Reworking subtitles.js to incorporate implementation of transcript display
 2) Started work on displaying transcripts
 3) Work halted because Panopto's SSL certs expired (omg, this is not the first time their system experienced a critical failure this summer…)</t>
+  </si>
+  <si>
+    <t>1) Implemented transcript tab megalist
+2) Added new slider options
+3) Removed webpack from package.json</t>
+  </si>
+  <si>
+    <t>1) Fixes to the flowplayer settings
+2) Modifications to transcript-display.js to include transcript sidebar
+3) Transcript side-bar implemented, yet to implement auto-scrolling and mini transcript sidebar</t>
+  </si>
+  <si>
+    <t>Meeting</t>
+  </si>
+  <si>
+    <t>1) Run through current state of project
+2) More discussion on HTML/CSS &amp; JS for Fyonn
+3) Discussion on design aspects</t>
+  </si>
+  <si>
+    <t>1) Misc fixes like fixes to the minimize / maximize button
+2) Added transcript tab on second screen tab
+3) Testing
+4) Added full-screen option
+5) Updated read me</t>
   </si>
 </sst>
 </file>
@@ -678,10 +703,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D66DA078-28E1-44A0-8117-A67A05B0BE09}">
-  <dimension ref="A1:F41"/>
+  <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1352,29 +1377,97 @@
         <v>56</v>
       </c>
     </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="C40" s="2" t="s">
+    <row r="40" spans="2:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B40" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C40" s="9">
+        <v>43661</v>
+      </c>
+      <c r="D40" s="2">
+        <v>6</v>
+      </c>
+      <c r="E40" s="2">
+        <v>0</v>
+      </c>
+      <c r="F40" s="11" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="B41" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C41" s="9">
+        <v>43664</v>
+      </c>
+      <c r="D41" s="2">
+        <v>8</v>
+      </c>
+      <c r="E41" s="2">
+        <v>0</v>
+      </c>
+      <c r="F41" s="11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B42" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="C42" s="9">
+        <v>43665</v>
+      </c>
+      <c r="D42" s="2">
+        <v>3</v>
+      </c>
+      <c r="E42" s="2">
+        <v>3</v>
+      </c>
+      <c r="F42" s="11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="B43" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C43" s="9">
+        <v>43666</v>
+      </c>
+      <c r="D43" s="2">
+        <v>6</v>
+      </c>
+      <c r="E43" s="2">
+        <v>0</v>
+      </c>
+      <c r="F43" s="11" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C44" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D40" s="3" t="s">
+      <c r="D44" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E40" s="3" t="s">
+      <c r="E44" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="C41" s="1">
-        <f>SUM(D41:E41)</f>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C45" s="1">
+        <f>SUM(D45:E45)</f>
+        <v>290</v>
+      </c>
+      <c r="D45" s="2">
+        <f>SUM(D3:D44)</f>
         <v>264</v>
       </c>
-      <c r="D41" s="2">
-        <f>SUM(D3:D40)</f>
-        <v>241</v>
-      </c>
-      <c r="E41" s="2">
-        <f>SUM(E3:E40)</f>
-        <v>23</v>
+      <c r="E45" s="2">
+        <f>SUM(E3:E44)</f>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated JSDocs, updated readme and project log, updated milestone 3 submission stuff
</commit_message>
<xml_diff>
--- a/Skylab documents/Project Log.xlsx
+++ b/Skylab documents/Project Log.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\Y1 Summer\Panopto Project\Skylab documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34E3C5A5-84AB-467C-8CB8-4FD36D2BE704}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EB2AE7A-3F72-4596-9494-1DDE91FE0260}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="5480" xr2:uid="{18F59187-B1E2-45ED-BF88-DDFCC51EE406}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{18F59187-B1E2-45ED-BF88-DDFCC51EE406}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="68">
   <si>
     <t>Project Log</t>
   </si>
@@ -305,6 +306,34 @@
 3) Testing
 4) Added full-screen option
 5) Updated read me</t>
+  </si>
+  <si>
+    <t>1) Preparation to upload to Chrome Webstore
+2) Icons
+3) Creating feature &amp; UI test rubrics</t>
+  </si>
+  <si>
+    <t>Testing &amp; Development</t>
+  </si>
+  <si>
+    <t>Milestone 3</t>
+  </si>
+  <si>
+    <t>1) Readme</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) Video
+2) Updating documents &amp; Chrome Webstore to reflect video URL
+3) Poster </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) Testing of features
+2) Testing of UI with focus group
+3) Fixes to bugs discovered during testing
+4) Include basic notifications to point users to settings page if they want to customize
+5) Improved settings page UI with tooltips and tweaks following feedback that it is too technical
+6) Updating app on Chrome Webstore
+7) Designing of the logo, taking of screenshots etc for chrome webstore </t>
   </si>
 </sst>
 </file>
@@ -703,10 +732,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D66DA078-28E1-44A0-8117-A67A05B0BE09}">
-  <dimension ref="A1:F45"/>
+  <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F43" sqref="F43"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F48" sqref="F47:F48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1445,28 +1474,96 @@
         <v>61</v>
       </c>
     </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="C44" s="2" t="s">
+    <row r="44" spans="2:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B44" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C44" s="9">
+        <v>43669</v>
+      </c>
+      <c r="D44" s="2">
+        <v>8</v>
+      </c>
+      <c r="E44" s="2">
+        <v>0</v>
+      </c>
+      <c r="F44" s="11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="B45" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="C45" s="9">
+        <v>43671</v>
+      </c>
+      <c r="D45" s="2">
+        <v>10</v>
+      </c>
+      <c r="E45" s="2">
+        <v>0</v>
+      </c>
+      <c r="F45" s="11" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B46" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="C46" s="9">
+        <v>43672</v>
+      </c>
+      <c r="D46" s="2">
+        <v>6</v>
+      </c>
+      <c r="E46" s="2">
+        <v>0</v>
+      </c>
+      <c r="F46" s="11" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B47" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="C47" s="9">
+        <v>43673</v>
+      </c>
+      <c r="D47" s="2">
+        <v>10</v>
+      </c>
+      <c r="E47" s="2">
+        <v>0</v>
+      </c>
+      <c r="F47" s="11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C48" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D44" s="3" t="s">
+      <c r="D48" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E44" s="3" t="s">
+      <c r="E48" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="C45" s="1">
-        <f>SUM(D45:E45)</f>
-        <v>290</v>
-      </c>
-      <c r="D45" s="2">
-        <f>SUM(D3:D44)</f>
-        <v>264</v>
-      </c>
-      <c r="E45" s="2">
-        <f>SUM(E3:E44)</f>
+    <row r="49" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C49" s="1">
+        <f>SUM(D49:E49)</f>
+        <v>324</v>
+      </c>
+      <c r="D49" s="2">
+        <f>SUM(D3:D48)</f>
+        <v>298</v>
+      </c>
+      <c r="E49" s="2">
+        <f>SUM(E3:E48)</f>
         <v>26</v>
       </c>
     </row>

</xml_diff>